<commit_message>
add autofill.xlsx update protection.xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/protection.xlsx
+++ b/src/main/webapp/book/protection.xlsx
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34460" yWindow="460" windowWidth="33600" windowHeight="20460"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="no operation" sheetId="5" r:id="rId1"/>
-    <sheet name="select" sheetId="15" r:id="rId2"/>
+    <sheet name="unlock" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="RangeMerged" localSheetId="1">#REF!</definedName>
     <definedName name="RangeMerged">#REF!</definedName>
+    <definedName name="TestRange1" localSheetId="1">#REF!</definedName>
     <definedName name="TestRange1">#REF!</definedName>
+    <definedName name="TestRange2" localSheetId="1">#REF!</definedName>
     <definedName name="TestRange2">#REF!</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -33,17 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>only cells with blue backgroud are editable (unlocked)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>the sheet is protected and allow selecting locked and unlocked cells</t>
+    <t>This sheet is protected and no actions allowed including cell selection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>This sheet is protected and no actions allowed including cell selection</t>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>try to unlock this sheet with</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,9 +432,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -432,7 +445,56 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+  </sheetData>
+  <sheetProtection password="CF11" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="3" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -459,28 +521,6 @@
       <c r="C4" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>